<commit_message>
Remove multistyled cells from cases 07, 10, and create case 12 for multistyle cells
</commit_message>
<xml_diff>
--- a/test/07_hyperlink_01.xlsx
+++ b/test/07_hyperlink_01.xlsx
@@ -24,26 +24,7 @@
     <t>Description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>double </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>quotation mark</t>
-    </r>
+    <t>double quotation mark</t>
   </si>
 </sst>
 </file>
@@ -66,7 +47,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -97,7 +78,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -404,7 +385,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>